<commit_message>
Report Export Correction with Total in  Footer
</commit_message>
<xml_diff>
--- a/sample/samplemachine.xlsx
+++ b/sample/samplemachine.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\cnc\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{63C3AC03-FCF3-4DE6-ADD0-10FB85861B16}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F72B9E6A-5C1B-47D7-A049-32A19CFFC04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="15600" windowHeight="7680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -236,15 +236,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>160242</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1676400</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>50669</xdr:rowOff>
+      <xdr:colOff>1447800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>147706</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -260,21 +260,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="57150" y="552450"/>
-          <a:ext cx="1619250" cy="450719"/>
+          <a:off x="160242" y="209550"/>
+          <a:ext cx="1287558" cy="1081156"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>